<commit_message>
Uploading the updated mosip master xlsx 1.2.0.1
Prepared the test data xlsx files for 1.2.0.1 mosip master.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/gender.xlsx
+++ b/mosip_master/xlsx/gender.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
   <si>
     <t xml:space="preserve">lang_code</t>
   </si>
@@ -83,42 +83,6 @@
   </si>
   <si>
     <t xml:space="preserve">آحرون</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ಪುರುಷ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ಹೆಣ್ಣು</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ಇತರರು</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">नर</t>
-  </si>
-  <si>
-    <t xml:space="preserve">महिला</t>
-  </si>
-  <si>
-    <t xml:space="preserve">अन्य</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ஆண்</t>
-  </si>
-  <si>
-    <t xml:space="preserve">பெண்</t>
-  </si>
-  <si>
-    <t xml:space="preserve">மற்றவைகள்</t>
   </si>
 </sst>
 </file>
@@ -251,10 +215,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -402,132 +366,6 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>